<commit_message>
added Mfa swagger yes
</commit_message>
<xml_diff>
--- a/documents/Zeitplan_DA11.xlsx
+++ b/documents/Zeitplan_DA11.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr showObjects="none"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Coding\DermaAI\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D542DD-0029-459F-9610-1D8666CADF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF7EA8-1F70-4C38-995D-33F5660BA239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E1416A3-E24D-4245-BA29-B5301C34C0E1}"/>
   </bookViews>
@@ -234,7 +234,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +273,13 @@
     <font>
       <sz val="11"/>
       <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="0.39997558519241921"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -859,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -941,6 +948,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -948,9 +964,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
@@ -965,12 +978,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1514,7 +1524,7 @@
   <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,37 +1561,37 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="67" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="62" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67" t="s">
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67" t="s">
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
       <c r="W1"/>
       <c r="AG1"/>
       <c r="AH1"/>
@@ -1863,8 +1873,8 @@
       <c r="J8" s="4"/>
       <c r="L8" s="49"/>
       <c r="M8" s="49"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="25"/>
@@ -1903,8 +1913,12 @@
       <c r="O9" s="8"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="9"/>
+      <c r="R9" s="71"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="72"/>
+      <c r="W9" s="73"/>
       <c r="X9" s="4"/>
       <c r="AB9" s="43"/>
       <c r="AC9" s="4"/>
@@ -1931,8 +1945,8 @@
       <c r="K10" s="49"/>
       <c r="L10" s="49"/>
       <c r="M10" s="49"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="68"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="8"/>
@@ -2088,12 +2102,12 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="69"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="60"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
@@ -2237,7 +2251,7 @@
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
       <c r="V19" s="13"/>
-      <c r="W19" s="70"/>
+      <c r="W19" s="61"/>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
       <c r="Z19" s="13"/>
@@ -2255,11 +2269,11 @@
       <c r="W20" s="9"/>
       <c r="AB20" s="9"/>
       <c r="AD20" s="46"/>
-      <c r="AE20" s="59" t="s">
+      <c r="AE20" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="AF20" s="60"/>
-      <c r="AG20" s="61"/>
+      <c r="AF20" s="65"/>
+      <c r="AG20" s="66"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E21" s="57"/>
@@ -2269,47 +2283,47 @@
       <c r="W21" s="9"/>
       <c r="AB21" s="9"/>
       <c r="AD21" s="47"/>
-      <c r="AE21" s="62" t="s">
+      <c r="AE21" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="AF21" s="62"/>
-      <c r="AG21" s="66"/>
+      <c r="AF21" s="63"/>
+      <c r="AG21" s="70"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E22" s="57"/>
       <c r="W22" s="9"/>
       <c r="AB22" s="9"/>
       <c r="AD22" s="48"/>
-      <c r="AE22" s="65" t="s">
+      <c r="AE22" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="AF22" s="62"/>
-      <c r="AG22" s="66"/>
+      <c r="AF22" s="63"/>
+      <c r="AG22" s="70"/>
     </row>
     <row r="23" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="57"/>
       <c r="W23" s="9"/>
       <c r="AB23" s="9"/>
       <c r="AD23" s="49"/>
-      <c r="AE23" s="63" t="s">
+      <c r="AE23" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="AF23" s="63"/>
-      <c r="AG23" s="64"/>
+      <c r="AF23" s="67"/>
+      <c r="AG23" s="68"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="D24" s="62" t="s">
+      <c r="D24" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="U24" s="62" t="s">
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="U24" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="V24" s="62"/>
-      <c r="W24" s="62"/>
-      <c r="X24" s="62"/>
-      <c r="Y24" s="62"/>
+      <c r="V24" s="63"/>
+      <c r="W24" s="63"/>
+      <c r="X24" s="63"/>
+      <c r="Y24" s="63"/>
       <c r="AB24" s="9"/>
       <c r="AG24" s="9"/>
     </row>
@@ -2336,23 +2350,18 @@
       <c r="AG30" s="9"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA31" s="62" t="s">
+      <c r="AA31" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="AB31" s="62"/>
-      <c r="AC31" s="62"/>
-      <c r="AD31" s="62"/>
-      <c r="AE31" s="62"/>
-      <c r="AF31" s="62"/>
-      <c r="AG31" s="62"/>
+      <c r="AB31" s="63"/>
+      <c r="AC31" s="63"/>
+      <c r="AD31" s="63"/>
+      <c r="AE31" s="63"/>
+      <c r="AF31" s="63"/>
+      <c r="AG31" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:R1"/>
     <mergeCell ref="AE20:AG20"/>
     <mergeCell ref="AA31:AG31"/>
     <mergeCell ref="D24:F24"/>
@@ -2360,6 +2369,11 @@
     <mergeCell ref="AE22:AG22"/>
     <mergeCell ref="AE21:AG21"/>
     <mergeCell ref="U24:Y24"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Praesi 3 und Diagramme hinzugefuegt.
</commit_message>
<xml_diff>
--- a/documents/Zeitplan_DA11.xlsx
+++ b/documents/Zeitplan_DA11.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showObjects="none"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Coding\DermaAI\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Programming\DermaAI\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF7EA8-1F70-4C38-995D-33F5660BA239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8D0568-A38E-4E6C-8382-A94006FD353C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E1416A3-E24D-4245-BA29-B5301C34C0E1}"/>
   </bookViews>
@@ -866,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -951,12 +951,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -964,6 +961,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
@@ -978,13 +978,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1524,7 +1527,7 @@
   <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,37 +1564,37 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="62" t="s">
+      <c r="C1" s="73"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="63" t="s">
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62" t="s">
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62" t="s">
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
       <c r="W1"/>
       <c r="AG1"/>
       <c r="AH1"/>
@@ -1913,12 +1916,12 @@
       <c r="O9" s="8"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
-      <c r="R9" s="71"/>
-      <c r="S9" s="71"/>
-      <c r="T9" s="71"/>
-      <c r="U9" s="71"/>
-      <c r="V9" s="72"/>
-      <c r="W9" s="73"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="64"/>
       <c r="X9" s="4"/>
       <c r="AB9" s="43"/>
       <c r="AC9" s="4"/>
@@ -1945,8 +1948,8 @@
       <c r="K10" s="49"/>
       <c r="L10" s="49"/>
       <c r="M10" s="49"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="8"/>
@@ -1981,8 +1984,12 @@
       <c r="K11" s="8"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="9"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="75"/>
+      <c r="W11" s="58"/>
       <c r="AB11" s="43"/>
       <c r="AC11" s="4"/>
       <c r="AF11" s="4"/>
@@ -2075,7 +2082,8 @@
       <c r="S14" s="8"/>
       <c r="V14" s="12"/>
       <c r="W14" s="9"/>
-      <c r="X14" s="4"/>
+      <c r="X14" s="74"/>
+      <c r="Y14" s="49"/>
       <c r="AB14" s="43"/>
       <c r="AC14" s="4"/>
       <c r="AG14" s="43"/>
@@ -2269,11 +2277,11 @@
       <c r="W20" s="9"/>
       <c r="AB20" s="9"/>
       <c r="AD20" s="46"/>
-      <c r="AE20" s="64" t="s">
+      <c r="AE20" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="AF20" s="65"/>
-      <c r="AG20" s="66"/>
+      <c r="AF20" s="66"/>
+      <c r="AG20" s="67"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E21" s="57"/>
@@ -2283,47 +2291,47 @@
       <c r="W21" s="9"/>
       <c r="AB21" s="9"/>
       <c r="AD21" s="47"/>
-      <c r="AE21" s="63" t="s">
+      <c r="AE21" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="AF21" s="63"/>
-      <c r="AG21" s="70"/>
+      <c r="AF21" s="68"/>
+      <c r="AG21" s="72"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E22" s="57"/>
       <c r="W22" s="9"/>
       <c r="AB22" s="9"/>
       <c r="AD22" s="48"/>
-      <c r="AE22" s="69" t="s">
+      <c r="AE22" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="AF22" s="63"/>
-      <c r="AG22" s="70"/>
+      <c r="AF22" s="68"/>
+      <c r="AG22" s="72"/>
     </row>
     <row r="23" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="57"/>
       <c r="W23" s="9"/>
       <c r="AB23" s="9"/>
       <c r="AD23" s="49"/>
-      <c r="AE23" s="67" t="s">
+      <c r="AE23" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="AF23" s="67"/>
-      <c r="AG23" s="68"/>
+      <c r="AF23" s="69"/>
+      <c r="AG23" s="70"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="D24" s="63" t="s">
+      <c r="D24" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="U24" s="63" t="s">
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="U24" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="V24" s="63"/>
-      <c r="W24" s="63"/>
-      <c r="X24" s="63"/>
-      <c r="Y24" s="63"/>
+      <c r="V24" s="68"/>
+      <c r="W24" s="68"/>
+      <c r="X24" s="68"/>
+      <c r="Y24" s="68"/>
       <c r="AB24" s="9"/>
       <c r="AG24" s="9"/>
     </row>
@@ -2350,18 +2358,23 @@
       <c r="AG30" s="9"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA31" s="63" t="s">
+      <c r="AA31" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="AB31" s="63"/>
-      <c r="AC31" s="63"/>
-      <c r="AD31" s="63"/>
-      <c r="AE31" s="63"/>
-      <c r="AF31" s="63"/>
-      <c r="AG31" s="63"/>
+      <c r="AB31" s="68"/>
+      <c r="AC31" s="68"/>
+      <c r="AD31" s="68"/>
+      <c r="AE31" s="68"/>
+      <c r="AF31" s="68"/>
+      <c r="AG31" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:R1"/>
     <mergeCell ref="AE20:AG20"/>
     <mergeCell ref="AA31:AG31"/>
     <mergeCell ref="D24:F24"/>
@@ -2369,11 +2382,6 @@
     <mergeCell ref="AE22:AG22"/>
     <mergeCell ref="AE21:AG21"/>
     <mergeCell ref="U24:Y24"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished ai model backend v1
</commit_message>
<xml_diff>
--- a/documents/Zeitplan_DA11.xlsx
+++ b/documents/Zeitplan_DA11.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showObjects="none"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Programming\DermaAI\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\GitHubClones\DermaAI\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8D0568-A38E-4E6C-8382-A94006FD353C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC91FE2-30C2-49A7-B3E9-11D047ECEAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E1416A3-E24D-4245-BA29-B5301C34C0E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6E1416A3-E24D-4245-BA29-B5301C34C0E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,7 +234,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,15 +277,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="6" tint="0.39997558519241921"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,12 +309,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="45">
     <border>
@@ -866,7 +853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -891,7 +878,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -942,18 +928,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -961,9 +950,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
@@ -978,16 +964,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1526,11 +1506,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F5C78B-75D0-448F-8E31-DF90C02D3391}">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
@@ -1564,37 +1544,37 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="73" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="68" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73" t="s">
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73" t="s">
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
       <c r="W1"/>
       <c r="AG1"/>
       <c r="AH1"/>
@@ -1615,7 +1595,7 @@
       <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="51" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1684,7 +1664,7 @@
       <c r="AA2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="42" t="s">
+      <c r="AB2" s="41" t="s">
         <v>32</v>
       </c>
       <c r="AC2" s="3" t="s">
@@ -1711,16 +1691,16 @@
       <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="29">
         <v>10</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <v>10</v>
       </c>
-      <c r="D3" s="50">
+      <c r="D3" s="49">
         <v>10</v>
       </c>
-      <c r="E3" s="53"/>
+      <c r="E3" s="48"/>
       <c r="H3" s="9"/>
       <c r="J3" s="4"/>
       <c r="P3" s="17"/>
@@ -1728,10 +1708,10 @@
       <c r="V3" s="12"/>
       <c r="W3" s="9"/>
       <c r="X3" s="4"/>
-      <c r="AB3" s="43"/>
+      <c r="AB3" s="42"/>
       <c r="AC3" s="4"/>
       <c r="AF3" s="4"/>
-      <c r="AG3" s="43"/>
+      <c r="AG3" s="42"/>
       <c r="AH3"/>
       <c r="AI3"/>
       <c r="AJ3"/>
@@ -1741,17 +1721,17 @@
       <c r="A4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="29">
         <v>20</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>10</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D4" s="49">
         <v>10</v>
       </c>
-      <c r="E4" s="54"/>
-      <c r="F4" s="8"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="12"/>
       <c r="H4" s="9"/>
       <c r="J4" s="4"/>
@@ -1760,10 +1740,10 @@
       <c r="V4" s="12"/>
       <c r="W4" s="9"/>
       <c r="X4" s="4"/>
-      <c r="AB4" s="43"/>
+      <c r="AB4" s="42"/>
       <c r="AC4" s="4"/>
       <c r="AF4" s="4"/>
-      <c r="AG4" s="43"/>
+      <c r="AG4" s="42"/>
       <c r="AH4"/>
       <c r="AI4"/>
       <c r="AJ4"/>
@@ -1773,29 +1753,29 @@
       <c r="A5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="29">
         <v>20</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>20</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="49">
         <v>25</v>
       </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="24"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="J5" s="4"/>
       <c r="P5" s="17"/>
       <c r="Q5" s="17"/>
       <c r="V5" s="12"/>
       <c r="W5" s="9"/>
       <c r="X5" s="4"/>
-      <c r="AB5" s="43"/>
+      <c r="AB5" s="42"/>
       <c r="AC5" s="4"/>
       <c r="AF5" s="4"/>
-      <c r="AG5" s="43"/>
+      <c r="AG5" s="42"/>
       <c r="AH5"/>
       <c r="AI5"/>
       <c r="AJ5"/>
@@ -1805,26 +1785,26 @@
       <c r="A6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="29">
         <v>30</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="55"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="53"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="17"/>
       <c r="V6" s="12"/>
       <c r="W6" s="9"/>
       <c r="X6" s="4"/>
-      <c r="AB6" s="43"/>
+      <c r="AB6" s="42"/>
       <c r="AC6" s="4"/>
       <c r="AF6" s="4"/>
-      <c r="AG6" s="43"/>
+      <c r="AG6" s="42"/>
       <c r="AH6"/>
       <c r="AI6"/>
       <c r="AJ6"/>
@@ -1834,29 +1814,29 @@
       <c r="A7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>40</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="53"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="17"/>
       <c r="V7" s="12"/>
       <c r="W7" s="9"/>
       <c r="X7" s="4"/>
-      <c r="AB7" s="43"/>
+      <c r="AB7" s="42"/>
       <c r="AC7" s="4"/>
       <c r="AF7" s="4"/>
-      <c r="AG7" s="43"/>
+      <c r="AG7" s="42"/>
       <c r="AH7"/>
       <c r="AI7"/>
       <c r="AJ7"/>
@@ -1866,31 +1846,31 @@
       <c r="A8" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>40</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="55"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="53"/>
       <c r="H8" s="9"/>
       <c r="J8" s="4"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="59"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="57"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="24"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
       <c r="X8" s="4"/>
-      <c r="AB8" s="43"/>
+      <c r="AB8" s="42"/>
       <c r="AC8" s="4"/>
       <c r="AF8" s="4"/>
-      <c r="AG8" s="43"/>
+      <c r="AG8" s="42"/>
       <c r="AH8"/>
       <c r="AI8"/>
       <c r="AJ8"/>
@@ -1900,12 +1880,12 @@
       <c r="A9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="31">
+      <c r="B9" s="32"/>
+      <c r="C9" s="30">
         <v>60</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="55"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="53"/>
       <c r="H9" s="9"/>
       <c r="I9" s="8"/>
       <c r="J9" s="7"/>
@@ -1916,17 +1896,21 @@
       <c r="O9" s="8"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="63"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="4"/>
-      <c r="AB9" s="43"/>
-      <c r="AC9" s="4"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="24"/>
       <c r="AF9" s="4"/>
-      <c r="AG9" s="43"/>
+      <c r="AG9" s="42"/>
       <c r="AH9"/>
       <c r="AI9"/>
       <c r="AJ9"/>
@@ -1936,33 +1920,33 @@
       <c r="A10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="31">
+      <c r="B10" s="32"/>
+      <c r="C10" s="30">
         <v>50</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="55"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="53"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="24"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="46"/>
+      <c r="V10" s="46"/>
+      <c r="W10" s="46"/>
       <c r="X10" s="4"/>
-      <c r="AB10" s="43"/>
+      <c r="AB10" s="42"/>
       <c r="AC10" s="4"/>
       <c r="AF10" s="4"/>
-      <c r="AG10" s="43"/>
+      <c r="AG10" s="42"/>
       <c r="AH10"/>
       <c r="AI10"/>
       <c r="AJ10"/>
@@ -1972,28 +1956,28 @@
       <c r="A11" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="50">
+      <c r="B11" s="31"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="49">
         <v>20</v>
       </c>
-      <c r="E11" s="55"/>
+      <c r="E11" s="53"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="8"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
-      <c r="U11" s="49"/>
-      <c r="V11" s="75"/>
-      <c r="W11" s="58"/>
-      <c r="AB11" s="43"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="56"/>
+      <c r="AB11" s="42"/>
       <c r="AC11" s="4"/>
       <c r="AF11" s="4"/>
-      <c r="AG11" s="43"/>
+      <c r="AG11" s="42"/>
       <c r="AH11"/>
       <c r="AI11"/>
       <c r="AJ11"/>
@@ -2003,27 +1987,27 @@
       <c r="A12" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="50">
+      <c r="B12" s="31"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="49">
         <v>30</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="53"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
       <c r="V12" s="12"/>
       <c r="W12" s="9"/>
       <c r="X12" s="4"/>
-      <c r="AB12" s="43"/>
+      <c r="AB12" s="42"/>
       <c r="AC12" s="4"/>
       <c r="AF12" s="4"/>
-      <c r="AG12" s="43"/>
+      <c r="AG12" s="42"/>
       <c r="AH12"/>
       <c r="AI12"/>
       <c r="AJ12"/>
@@ -2033,27 +2017,29 @@
       <c r="A13" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="50">
+      <c r="B13" s="28"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="49">
         <v>10</v>
       </c>
-      <c r="E13" s="55"/>
+      <c r="E13" s="53"/>
       <c r="H13" s="9"/>
       <c r="J13" s="4"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="8"/>
-      <c r="AB13" s="43"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="AB13" s="42"/>
       <c r="AC13" s="4"/>
       <c r="AF13"/>
       <c r="AG13" s="9"/>
@@ -2066,27 +2052,29 @@
       <c r="A14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="50">
+      <c r="B14" s="28"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="49">
         <v>10</v>
       </c>
-      <c r="E14" s="55"/>
+      <c r="E14" s="53"/>
       <c r="H14" s="9"/>
       <c r="J14" s="4"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="17"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="74"/>
-      <c r="Y14" s="49"/>
-      <c r="AB14" s="43"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="48"/>
+      <c r="V14" s="48"/>
+      <c r="W14" s="48"/>
+      <c r="X14" s="59"/>
+      <c r="Y14" s="48"/>
+      <c r="AB14" s="42"/>
       <c r="AC14" s="4"/>
-      <c r="AG14" s="43"/>
+      <c r="AG14" s="42"/>
       <c r="AH14"/>
       <c r="AI14"/>
       <c r="AJ14"/>
@@ -2096,12 +2084,12 @@
       <c r="A15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="50">
+      <c r="B15" s="28"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="49">
         <v>20</v>
       </c>
-      <c r="E15" s="55"/>
+      <c r="E15" s="53"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="9"/>
@@ -2110,21 +2098,21 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="60"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="24"/>
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="48"/>
+      <c r="U15" s="48"/>
+      <c r="V15" s="48"/>
+      <c r="W15" s="48"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
-      <c r="AB15" s="43"/>
+      <c r="AB15" s="42"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
@@ -2135,12 +2123,12 @@
       <c r="A16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="50">
+      <c r="B16" s="33"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="49">
         <v>30</v>
       </c>
-      <c r="E16" s="55"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="9"/>
@@ -2163,7 +2151,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="8"/>
       <c r="AA16" s="8"/>
-      <c r="AB16" s="44"/>
+      <c r="AB16" s="43"/>
       <c r="AC16" s="4"/>
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
@@ -2178,16 +2166,16 @@
       <c r="A17" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="28">
         <v>30</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="27">
         <v>30</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="50">
         <v>30</v>
       </c>
-      <c r="E17" s="56"/>
+      <c r="E17" s="54"/>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
       <c r="H17" s="9"/>
@@ -2210,42 +2198,42 @@
       <c r="Y17" s="20"/>
       <c r="Z17" s="20"/>
       <c r="AA17" s="20"/>
-      <c r="AB17" s="45"/>
-      <c r="AC17" s="41"/>
-      <c r="AD17" s="26"/>
-      <c r="AE17" s="26"/>
-      <c r="AF17" s="26"/>
-      <c r="AG17" s="44"/>
+      <c r="AB17" s="44"/>
+      <c r="AC17" s="40"/>
+      <c r="AD17" s="25"/>
+      <c r="AE17" s="25"/>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="43"/>
     </row>
     <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="35"/>
-      <c r="E18" s="57"/>
+      <c r="B18" s="34"/>
+      <c r="E18" s="55"/>
       <c r="H18" s="9"/>
       <c r="W18" s="9"/>
       <c r="AB18" s="9"/>
       <c r="AG18" s="9"/>
     </row>
     <row r="19" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="36">
+      <c r="B19" s="35">
         <f>SUM(B3:B17)</f>
         <v>190</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="26">
         <f>SUM(C3:C17)</f>
         <v>180</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="26">
         <f>SUM(D3:D17)</f>
         <v>195</v>
       </c>
-      <c r="E19" s="40"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="40"/>
+      <c r="I19" s="39"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
@@ -2259,79 +2247,79 @@
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
       <c r="V19" s="13"/>
-      <c r="W19" s="61"/>
+      <c r="W19" s="58"/>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
       <c r="Z19" s="13"/>
       <c r="AA19" s="13"/>
       <c r="AB19" s="14"/>
       <c r="AC19" s="13"/>
-      <c r="AD19" s="37"/>
-      <c r="AE19" s="37"/>
-      <c r="AF19" s="37"/>
-      <c r="AG19" s="39"/>
+      <c r="AD19" s="36"/>
+      <c r="AE19" s="36"/>
+      <c r="AF19" s="36"/>
+      <c r="AG19" s="38"/>
     </row>
     <row r="20" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="57"/>
-      <c r="H20" s="39"/>
+      <c r="E20" s="55"/>
+      <c r="H20" s="38"/>
       <c r="W20" s="9"/>
       <c r="AB20" s="9"/>
-      <c r="AD20" s="46"/>
-      <c r="AE20" s="65" t="s">
+      <c r="AD20" s="45"/>
+      <c r="AE20" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="AF20" s="66"/>
-      <c r="AG20" s="67"/>
+      <c r="AF20" s="64"/>
+      <c r="AG20" s="65"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="E21" s="57"/>
+      <c r="E21" s="55"/>
       <c r="F21" t="s">
         <v>62</v>
       </c>
       <c r="W21" s="9"/>
       <c r="AB21" s="9"/>
-      <c r="AD21" s="47"/>
-      <c r="AE21" s="68" t="s">
+      <c r="AD21" s="46"/>
+      <c r="AE21" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="AF21" s="68"/>
-      <c r="AG21" s="72"/>
+      <c r="AF21" s="62"/>
+      <c r="AG21" s="69"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="E22" s="57"/>
+      <c r="E22" s="55"/>
       <c r="W22" s="9"/>
       <c r="AB22" s="9"/>
-      <c r="AD22" s="48"/>
-      <c r="AE22" s="71" t="s">
+      <c r="AD22" s="47"/>
+      <c r="AE22" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="AF22" s="68"/>
-      <c r="AG22" s="72"/>
+      <c r="AF22" s="62"/>
+      <c r="AG22" s="69"/>
     </row>
     <row r="23" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="57"/>
+      <c r="E23" s="55"/>
       <c r="W23" s="9"/>
       <c r="AB23" s="9"/>
-      <c r="AD23" s="49"/>
-      <c r="AE23" s="69" t="s">
+      <c r="AD23" s="48"/>
+      <c r="AE23" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="AF23" s="69"/>
-      <c r="AG23" s="70"/>
+      <c r="AF23" s="66"/>
+      <c r="AG23" s="67"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="D24" s="68" t="s">
+      <c r="D24" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="U24" s="68" t="s">
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="U24" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="V24" s="68"/>
-      <c r="W24" s="68"/>
-      <c r="X24" s="68"/>
-      <c r="Y24" s="68"/>
+      <c r="V24" s="62"/>
+      <c r="W24" s="62"/>
+      <c r="X24" s="62"/>
+      <c r="Y24" s="62"/>
       <c r="AB24" s="9"/>
       <c r="AG24" s="9"/>
     </row>
@@ -2358,23 +2346,18 @@
       <c r="AG30" s="9"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA31" s="68" t="s">
+      <c r="AA31" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="AB31" s="68"/>
-      <c r="AC31" s="68"/>
-      <c r="AD31" s="68"/>
-      <c r="AE31" s="68"/>
-      <c r="AF31" s="68"/>
-      <c r="AG31" s="68"/>
+      <c r="AB31" s="62"/>
+      <c r="AC31" s="62"/>
+      <c r="AD31" s="62"/>
+      <c r="AE31" s="62"/>
+      <c r="AF31" s="62"/>
+      <c r="AG31" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:R1"/>
     <mergeCell ref="AE20:AG20"/>
     <mergeCell ref="AA31:AG31"/>
     <mergeCell ref="D24:F24"/>
@@ -2382,6 +2365,11 @@
     <mergeCell ref="AE22:AG22"/>
     <mergeCell ref="AE21:AG21"/>
     <mergeCell ref="U24:Y24"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>